<commit_message>
Revised version of Form 3-BU
</commit_message>
<xml_diff>
--- a/forms/Form-3BU.xlsx
+++ b/forms/Form-3BU.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\bitbucket_workspaces\IOTC-ws\R libs\workflow\forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D85CB70-66A9-4532-8859-9928A8CFEEA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0DF6046-ECC5-47BD-992B-761141E1FE30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="GFpj//VivYAPeIU08ZJg1Dux9toxRhSuIx/DIcXzwdN7RVpS32MIopnBIf/zfwa+hDKrfFh8CXTLPmmG/7iI6w==" workbookSaltValue="5rYiPYrZuKGJOy5hPiufCQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{742ED9EC-8AD9-42B2-9B99-191B35B67816}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{742ED9EC-8AD9-42B2-9B99-191B35B67816}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -1020,8 +1020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC2D41B5-AC8B-4133-9C08-EAF515BF72F5}">
   <dimension ref="B1:H32"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1384,11 +1384,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C098252-FABC-4161-882E-794F98E79BC6}">
   <dimension ref="B1:E55"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Minor fixes to 3BU.xlsx
</commit_message>
<xml_diff>
--- a/forms/Form-3BU.xlsx
+++ b/forms/Form-3BU.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\bitbucket_workspaces\IOTC-ws\R libs\workflow\forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0DF6046-ECC5-47BD-992B-761141E1FE30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D3F648-F5AC-47EE-8446-BBEE61A3CD2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="GFpj//VivYAPeIU08ZJg1Dux9toxRhSuIx/DIcXzwdN7RVpS32MIopnBIf/zfwa+hDKrfFh8CXTLPmmG/7iI6w==" workbookSaltValue="5rYiPYrZuKGJOy5hPiufCQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{742ED9EC-8AD9-42B2-9B99-191B35B67816}"/>
+    <workbookView xWindow="34305" yWindow="2610" windowWidth="21600" windowHeight="11295" xr2:uid="{742ED9EC-8AD9-42B2-9B99-191B35B67816}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -1020,8 +1020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC2D41B5-AC8B-4133-9C08-EAF515BF72F5}">
   <dimension ref="B1:H32"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1384,11 +1384,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C098252-FABC-4161-882E-794F98E79BC6}">
   <dimension ref="B1:E55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>